<commit_message>
yeah we needed that
</commit_message>
<xml_diff>
--- a/thrustCurveData.xlsx
+++ b/thrustCurveData.xlsx
@@ -424,14 +424,489 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
       <selection activeCell="E23" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>EndTime</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Slope</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Intercept</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="B2" t="n">
+        <v>52.42857142857142</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="B3" t="n">
+        <v>101.4925373134328</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-2.404134328358209</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.184</v>
+      </c>
+      <c r="B4" t="n">
+        <v>116.2647058823529</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-4.117705882352944</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="B5" t="n">
+        <v>131.7547169811321</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-6.96786792452831</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.282</v>
+      </c>
+      <c r="B6" t="n">
+        <v>121.6000000000001</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-4.561200000000017</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.297</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-181.3333333333331</v>
+      </c>
+      <c r="C7" t="n">
+        <v>80.86599999999993</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.311</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-315.7857142857142</v>
+      </c>
+      <c r="C8" t="n">
+        <v>120.7983571428571</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.322</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-418.0909090909087</v>
+      </c>
+      <c r="C9" t="n">
+        <v>152.6152727272726</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.348</v>
+      </c>
+      <c r="B10" t="n">
+        <v>-148.6153846153848</v>
+      </c>
+      <c r="C10" t="n">
+        <v>65.84415384615389</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.386</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-53.34210526315783</v>
+      </c>
+      <c r="C11" t="n">
+        <v>32.68905263157892</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="B12" t="n">
+        <v>-23.05357142857144</v>
+      </c>
+      <c r="C12" t="n">
+        <v>20.99767857142858</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.546</v>
+      </c>
+      <c r="B13" t="n">
+        <v>-8.961538461538462</v>
+      </c>
+      <c r="C13" t="n">
+        <v>14.769</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0.718</v>
+      </c>
+      <c r="B14" t="n">
+        <v>-3.313953488372096</v>
+      </c>
+      <c r="C14" t="n">
+        <v>11.68541860465116</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0.879</v>
+      </c>
+      <c r="B15" t="n">
+        <v>-1.248447204968936</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10.2023850931677</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.066</v>
+      </c>
+      <c r="B16" t="n">
+        <v>-1.090909090909094</v>
+      </c>
+      <c r="C16" t="n">
+        <v>10.06390909090909</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1.257</v>
+      </c>
+      <c r="B17" t="n">
+        <v>-1.062827225130888</v>
+      </c>
+      <c r="C17" t="n">
+        <v>10.03397382198953</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.436</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-2.167597765363127</v>
+      </c>
+      <c r="C18" t="n">
+        <v>11.42267039106145</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="B19" t="n">
+        <v>-0.1038961038961039</v>
+      </c>
+      <c r="C19" t="n">
+        <v>8.459194805194805</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.612</v>
+      </c>
+      <c r="B20" t="n">
+        <v>-167.3181818181817</v>
+      </c>
+      <c r="C20" t="n">
+        <v>274.3299090909089</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-121.3947368421059</v>
+      </c>
+      <c r="C21" t="n">
+        <v>200.3013157894747</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>EndTime</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Slope</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Intercept</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="B23" t="n">
+        <v>52.42857142857142</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="B24" t="n">
+        <v>101.4925373134328</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-2.404134328358209</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0.184</v>
+      </c>
+      <c r="B25" t="n">
+        <v>116.2647058823529</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-4.117705882352944</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="B26" t="n">
+        <v>131.7547169811321</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-6.96786792452831</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>0.282</v>
+      </c>
+      <c r="B27" t="n">
+        <v>121.6000000000001</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-4.561200000000017</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>0.297</v>
+      </c>
+      <c r="B28" t="n">
+        <v>-181.3333333333331</v>
+      </c>
+      <c r="C28" t="n">
+        <v>80.86599999999993</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>0.311</v>
+      </c>
+      <c r="B29" t="n">
+        <v>-315.7857142857142</v>
+      </c>
+      <c r="C29" t="n">
+        <v>120.7983571428571</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0.322</v>
+      </c>
+      <c r="B30" t="n">
+        <v>-418.0909090909087</v>
+      </c>
+      <c r="C30" t="n">
+        <v>152.6152727272726</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>0.348</v>
+      </c>
+      <c r="B31" t="n">
+        <v>-148.6153846153848</v>
+      </c>
+      <c r="C31" t="n">
+        <v>65.84415384615389</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>0.386</v>
+      </c>
+      <c r="B32" t="n">
+        <v>-53.34210526315783</v>
+      </c>
+      <c r="C32" t="n">
+        <v>32.68905263157892</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="B33" t="n">
+        <v>-23.05357142857144</v>
+      </c>
+      <c r="C33" t="n">
+        <v>20.99767857142858</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0.546</v>
+      </c>
+      <c r="B34" t="n">
+        <v>-8.961538461538462</v>
+      </c>
+      <c r="C34" t="n">
+        <v>14.769</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>0.718</v>
+      </c>
+      <c r="B35" t="n">
+        <v>-3.313953488372096</v>
+      </c>
+      <c r="C35" t="n">
+        <v>11.68541860465116</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>0.879</v>
+      </c>
+      <c r="B36" t="n">
+        <v>-1.248447204968936</v>
+      </c>
+      <c r="C36" t="n">
+        <v>10.2023850931677</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1.066</v>
+      </c>
+      <c r="B37" t="n">
+        <v>-1.090909090909094</v>
+      </c>
+      <c r="C37" t="n">
+        <v>10.06390909090909</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1.257</v>
+      </c>
+      <c r="B38" t="n">
+        <v>-1.062827225130888</v>
+      </c>
+      <c r="C38" t="n">
+        <v>10.03397382198953</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1.436</v>
+      </c>
+      <c r="B39" t="n">
+        <v>-2.167597765363127</v>
+      </c>
+      <c r="C39" t="n">
+        <v>11.42267039106145</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="B40" t="n">
+        <v>-0.1038961038961039</v>
+      </c>
+      <c r="C40" t="n">
+        <v>8.459194805194805</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1.612</v>
+      </c>
+      <c r="B41" t="n">
+        <v>-167.3181818181817</v>
+      </c>
+      <c r="C41" t="n">
+        <v>274.3299090909089</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="B42" t="n">
+        <v>-121.3947368421059</v>
+      </c>
+      <c r="C42" t="n">
+        <v>200.3013157894747</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>